<commit_message>
fix: update Russia adm1 regex rules
</commit_message>
<xml_diff>
--- a/inst/extdata/countrycodes/russia_adm1.xlsx
+++ b/inst/extdata/countrycodes/russia_adm1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascalburkhard/Dropbox/Work/Geography/Visualization/R/Projects/Packages/geotools/inst/extdata/countrycodes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascalburkhard/Dropbox/Work/Geography/Visualization/R/Packages/geotools/inst/extdata/countrycodes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A1B597-A397-F24E-AEFC-44ABAB1C2A80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6735FC56-6F46-F042-9D7E-7FE86A2BBD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gks_yearbook_russia_adm1" sheetId="1" r:id="rId1"/>
@@ -541,9 +541,6 @@
     <t>RUS-2605</t>
   </si>
   <si>
-    <t>Tyva Republic</t>
-  </si>
-  <si>
     <t>Республика Тыва</t>
   </si>
   <si>
@@ -1765,9 +1762,6 @@
     <t>tyumen</t>
   </si>
   <si>
-    <t>tyva</t>
-  </si>
-  <si>
     <t>udmurtia</t>
   </si>
   <si>
@@ -2111,6 +2105,12 @@
   </si>
   <si>
     <t>(?:H|н)ижегородская</t>
+  </si>
+  <si>
+    <t>Tuva Republic</t>
+  </si>
+  <si>
+    <t>tuva|tyva</t>
   </si>
 </sst>
 </file>
@@ -2656,9 +2656,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2696,7 +2696,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2802,7 +2802,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2944,7 +2944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2954,8 +2954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2971,210 +2971,210 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E1" t="s">
+        <v>503</v>
+      </c>
+      <c r="F1" t="s">
         <v>504</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>505</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>506</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>507</v>
-      </c>
-      <c r="I1" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="H2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F3" t="s">
         <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F4" t="s">
         <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="H4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5" t="s">
         <v>100</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D5" t="s">
         <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F5" t="s">
         <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="H5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B6" t="s">
         <v>144</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F6" t="s">
         <v>145</v>
       </c>
       <c r="G6" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="H6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B7" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F7" t="s">
         <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="H7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -3183,56 +3183,56 @@
         <v>10000000000</v>
       </c>
       <c r="D8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="H8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="H9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B10" t="s">
         <v>81</v>
@@ -3244,24 +3244,24 @@
         <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F10" t="s">
         <v>83</v>
       </c>
       <c r="G10" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="H10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -3270,27 +3270,27 @@
         <v>12000000000</v>
       </c>
       <c r="D11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E11" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="H11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -3299,27 +3299,27 @@
         <v>14000000000</v>
       </c>
       <c r="D12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="H12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -3328,143 +3328,143 @@
         <v>15000000000</v>
       </c>
       <c r="D13" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E13" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="H13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I13" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C14" s="1">
         <v>17000000000</v>
       </c>
       <c r="D14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E14" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G14" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I14" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C15" s="1">
         <v>18000000000</v>
       </c>
       <c r="D15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E15" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G15" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="H15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C16" s="1">
         <v>19000000000</v>
       </c>
       <c r="D16" t="s">
+        <v>379</v>
+      </c>
+      <c r="E16" t="s">
+        <v>584</v>
+      </c>
+      <c r="F16" t="s">
+        <v>183</v>
+      </c>
+      <c r="G16" t="s">
+        <v>673</v>
+      </c>
+      <c r="H16" t="s">
         <v>380</v>
       </c>
-      <c r="E16" t="s">
-        <v>586</v>
-      </c>
-      <c r="F16" t="s">
-        <v>184</v>
-      </c>
-      <c r="G16" t="s">
-        <v>675</v>
-      </c>
-      <c r="H16" t="s">
-        <v>381</v>
-      </c>
       <c r="I16" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C17" s="1">
         <v>20000000000</v>
       </c>
       <c r="D17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E17" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G17" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="H17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B18" t="s">
         <v>84</v>
@@ -3473,27 +3473,27 @@
         <v>22000000000</v>
       </c>
       <c r="D18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E18" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F18" t="s">
         <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="H18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I18" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
@@ -3502,27 +3502,27 @@
         <v>24000000000</v>
       </c>
       <c r="D19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E19" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F19" t="s">
         <v>28</v>
       </c>
       <c r="G19" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="H19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -3531,27 +3531,27 @@
         <v>25000000000</v>
       </c>
       <c r="D20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E20" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F20" t="s">
         <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="H20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B21" t="s">
         <v>154</v>
@@ -3560,27 +3560,27 @@
         <v>26000000000</v>
       </c>
       <c r="D21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E21" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F21" t="s">
         <v>155</v>
       </c>
       <c r="G21" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="H21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B22" t="s">
         <v>33</v>
@@ -3589,27 +3589,27 @@
         <v>27000000000</v>
       </c>
       <c r="D22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E22" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I22" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B23" t="s">
         <v>168</v>
@@ -3618,27 +3618,27 @@
         <v>28000000000</v>
       </c>
       <c r="D23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E23" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F23" t="s">
         <v>169</v>
       </c>
       <c r="G23" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="H23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I23" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B24" t="s">
         <v>35</v>
@@ -3647,27 +3647,27 @@
         <v>29000000000</v>
       </c>
       <c r="D24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E24" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F24" t="s">
         <v>36</v>
       </c>
       <c r="G24" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="H24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I24" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B25" t="s">
         <v>37</v>
@@ -3679,53 +3679,53 @@
         <v>38</v>
       </c>
       <c r="E25" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F25" t="s">
         <v>39</v>
       </c>
       <c r="G25" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="H25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I25" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E26" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F26" t="s">
         <v>44</v>
       </c>
       <c r="G26" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="H26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I26" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B27" t="s">
         <v>50</v>
@@ -3734,27 +3734,27 @@
         <v>33000000000</v>
       </c>
       <c r="D27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F27" t="s">
         <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="H27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B28" t="s">
         <v>55</v>
@@ -3763,27 +3763,27 @@
         <v>34000000000</v>
       </c>
       <c r="D28" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F28" t="s">
         <v>56</v>
       </c>
       <c r="G28" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="H28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B29" t="s">
         <v>111</v>
@@ -3795,24 +3795,24 @@
         <v>112</v>
       </c>
       <c r="E29" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F29" t="s">
         <v>113</v>
       </c>
       <c r="G29" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="H29" t="s">
+        <v>545</v>
+      </c>
+      <c r="I29" t="s">
         <v>546</v>
-      </c>
-      <c r="I29" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B30" t="s">
         <v>133</v>
@@ -3821,27 +3821,27 @@
         <v>36000000000</v>
       </c>
       <c r="D30" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E30" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F30" t="s">
         <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="H30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I30" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B31" t="s">
         <v>61</v>
@@ -3850,27 +3850,27 @@
         <v>37000000000</v>
       </c>
       <c r="D31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E31" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F31" t="s">
         <v>62</v>
       </c>
       <c r="G31" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B32" t="s">
         <v>63</v>
@@ -3879,27 +3879,27 @@
         <v>38000000000</v>
       </c>
       <c r="D32" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E32" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
       </c>
       <c r="G32" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="H32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I32" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B33" t="s">
         <v>142</v>
@@ -3908,27 +3908,27 @@
         <v>40000000000</v>
       </c>
       <c r="D33" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E33" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F33" t="s">
         <v>143</v>
       </c>
       <c r="G33" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="H33" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I33" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B34" t="s">
         <v>65</v>
@@ -3937,27 +3937,27 @@
         <v>41000000000</v>
       </c>
       <c r="D34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E34" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F34" t="s">
         <v>66</v>
       </c>
       <c r="G34" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I34" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B35" t="s">
         <v>67</v>
@@ -3966,27 +3966,27 @@
         <v>42000000000</v>
       </c>
       <c r="D35" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E35" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F35" t="s">
         <v>68</v>
       </c>
       <c r="G35" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="H35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I35" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B36" t="s">
         <v>69</v>
@@ -3995,27 +3995,27 @@
         <v>44000000000</v>
       </c>
       <c r="D36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E36" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F36" t="s">
         <v>70</v>
       </c>
       <c r="G36" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="H36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I36" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B37" t="s">
         <v>74</v>
@@ -4027,24 +4027,24 @@
         <v>75</v>
       </c>
       <c r="E37" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F37" t="s">
         <v>76</v>
       </c>
       <c r="G37" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H37" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I37" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B38" t="s">
         <v>77</v>
@@ -4053,27 +4053,27 @@
         <v>46000000000</v>
       </c>
       <c r="D38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E38" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F38" t="s">
         <v>78</v>
       </c>
       <c r="G38" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I38" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B39" t="s">
         <v>79</v>
@@ -4082,27 +4082,27 @@
         <v>47000000000</v>
       </c>
       <c r="D39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E39" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F39" t="s">
         <v>80</v>
       </c>
       <c r="G39" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="H39" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I39" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B40" t="s">
         <v>86</v>
@@ -4111,27 +4111,27 @@
         <v>49000000000</v>
       </c>
       <c r="D40" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E40" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F40" t="s">
         <v>87</v>
       </c>
       <c r="G40" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="H40" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I40" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B41" t="s">
         <v>88</v>
@@ -4140,27 +4140,27 @@
         <v>50000000000</v>
       </c>
       <c r="D41" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F41" t="s">
         <v>89</v>
       </c>
       <c r="G41" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H41" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I41" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B42" t="s">
         <v>90</v>
@@ -4169,27 +4169,27 @@
         <v>52000000000</v>
       </c>
       <c r="D42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E42" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F42" t="s">
         <v>91</v>
       </c>
       <c r="G42" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="H42" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B43" t="s">
         <v>92</v>
@@ -4198,27 +4198,27 @@
         <v>53000000000</v>
       </c>
       <c r="D43" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E43" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F43" t="s">
         <v>93</v>
       </c>
       <c r="G43" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="H43" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I43" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B44" t="s">
         <v>94</v>
@@ -4227,27 +4227,27 @@
         <v>54000000000</v>
       </c>
       <c r="D44" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E44" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F44" t="s">
         <v>95</v>
       </c>
       <c r="G44" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="H44" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I44" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B45" t="s">
         <v>96</v>
@@ -4256,27 +4256,27 @@
         <v>56000000000</v>
       </c>
       <c r="D45" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E45" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F45" t="s">
         <v>97</v>
       </c>
       <c r="G45" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="H45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I45" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B46" t="s">
         <v>98</v>
@@ -4285,27 +4285,27 @@
         <v>57000000000</v>
       </c>
       <c r="D46" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E46" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F46" t="s">
         <v>99</v>
       </c>
       <c r="G46" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="H46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I46" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B47" t="s">
         <v>103</v>
@@ -4314,27 +4314,27 @@
         <v>58000000000</v>
       </c>
       <c r="D47" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E47" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F47" t="s">
         <v>104</v>
       </c>
       <c r="G47" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="H47" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I47" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B48" t="s">
         <v>126</v>
@@ -4343,27 +4343,27 @@
         <v>60000000000</v>
       </c>
       <c r="D48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E48" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F48" t="s">
         <v>127</v>
       </c>
       <c r="G48" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="H48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I48" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B49" t="s">
         <v>128</v>
@@ -4375,24 +4375,24 @@
         <v>129</v>
       </c>
       <c r="E49" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F49" t="s">
         <v>130</v>
       </c>
       <c r="G49" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="H49" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I49" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B50" t="s">
         <v>135</v>
@@ -4401,27 +4401,27 @@
         <v>63000000000</v>
       </c>
       <c r="D50" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E50" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F50" t="s">
         <v>136</v>
       </c>
       <c r="G50" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H50" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B51" t="s">
         <v>131</v>
@@ -4430,27 +4430,27 @@
         <v>64000000000</v>
       </c>
       <c r="D51" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E51" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F51" t="s">
         <v>132</v>
       </c>
       <c r="G51" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="H51" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I51" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B52" t="s">
         <v>146</v>
@@ -4459,27 +4459,27 @@
         <v>65000000000</v>
       </c>
       <c r="D52" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E52" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F52" t="s">
         <v>147</v>
       </c>
       <c r="G52" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H52" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I52" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B53" t="s">
         <v>140</v>
@@ -4488,27 +4488,27 @@
         <v>66000000000</v>
       </c>
       <c r="D53" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E53" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F53" t="s">
         <v>141</v>
       </c>
       <c r="G53" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="H53" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I53" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B54" t="s">
         <v>137</v>
@@ -4520,24 +4520,24 @@
         <v>138</v>
       </c>
       <c r="E54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F54" t="s">
         <v>139</v>
       </c>
       <c r="G54" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="H54" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I54" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B55" t="s">
         <v>148</v>
@@ -4546,27 +4546,27 @@
         <v>68000000000</v>
       </c>
       <c r="D55" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E55" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F55" t="s">
         <v>149</v>
       </c>
       <c r="G55" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="H55" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I55" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B56" t="s">
         <v>162</v>
@@ -4575,27 +4575,27 @@
         <v>69000000000</v>
       </c>
       <c r="D56" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E56" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F56" t="s">
         <v>163</v>
       </c>
       <c r="G56" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="H56" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I56" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B57" t="s">
         <v>166</v>
@@ -4604,56 +4604,56 @@
         <v>70000000000</v>
       </c>
       <c r="D57" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E57" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F57" t="s">
         <v>167</v>
       </c>
       <c r="G57" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="H57" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I57" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B58" t="s">
         <v>170</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D58" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E58" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F58" t="s">
         <v>171</v>
       </c>
       <c r="G58" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="H58" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I58" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B59" t="s">
         <v>47</v>
@@ -4665,82 +4665,82 @@
         <v>48</v>
       </c>
       <c r="E59" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F59" t="s">
         <v>49</v>
       </c>
       <c r="G59" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="H59" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I59" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C60" s="1">
         <v>71140000000</v>
       </c>
       <c r="D60" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E60" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F60" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G60" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="H60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I60" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B61" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C61" s="1">
         <v>73000000000</v>
       </c>
       <c r="D61" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E61" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F61" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G61" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H61" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I61" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B62" t="s">
         <v>18</v>
@@ -4749,27 +4749,27 @@
         <v>75000000000</v>
       </c>
       <c r="D62" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E62" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F62" t="s">
         <v>19</v>
       </c>
       <c r="G62" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="H62" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I62" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B63" t="s">
         <v>164</v>
@@ -4778,27 +4778,27 @@
         <v>76000000000</v>
       </c>
       <c r="D63" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E63" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F63" t="s">
         <v>165</v>
       </c>
       <c r="G63" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H63" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I63" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B64" t="s">
         <v>20</v>
@@ -4807,56 +4807,56 @@
         <v>77000000000</v>
       </c>
       <c r="D64" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E64" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F64" t="s">
         <v>21</v>
       </c>
       <c r="G64" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="H64" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I64" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C65" s="1">
         <v>78000000000</v>
       </c>
       <c r="D65" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E65" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G65" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="H65" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I65" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B66" t="s">
         <v>105</v>
@@ -4868,24 +4868,24 @@
         <v>106</v>
       </c>
       <c r="E66" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F66" t="s">
         <v>107</v>
       </c>
       <c r="G66" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H66" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I66" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B67" t="s">
         <v>108</v>
@@ -4897,24 +4897,24 @@
         <v>109</v>
       </c>
       <c r="E67" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F67" t="s">
         <v>110</v>
       </c>
       <c r="G67" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="H67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I67" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B68" t="s">
         <v>150</v>
@@ -4923,27 +4923,27 @@
         <v>81000000000</v>
       </c>
       <c r="D68" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E68" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F68" t="s">
         <v>151</v>
       </c>
       <c r="G68" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H68" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I68" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B69" t="s">
         <v>152</v>
@@ -4952,27 +4952,27 @@
         <v>82000000000</v>
       </c>
       <c r="D69" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E69" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F69" t="s">
         <v>153</v>
       </c>
       <c r="G69" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H69" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I69" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B70" t="s">
         <v>31</v>
@@ -4981,27 +4981,27 @@
         <v>83000000000</v>
       </c>
       <c r="D70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E70" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F70" t="s">
         <v>32</v>
       </c>
       <c r="G70" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="H70" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I70" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B71" t="s">
         <v>2</v>
@@ -5013,24 +5013,24 @@
         <v>3</v>
       </c>
       <c r="E71" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F71" t="s">
         <v>4</v>
       </c>
       <c r="G71" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="H71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I71" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B72" t="s">
         <v>114</v>
@@ -5042,24 +5042,24 @@
         <v>115</v>
       </c>
       <c r="E72" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F72" t="s">
         <v>116</v>
       </c>
       <c r="G72" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="H72" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I72" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B73" t="s">
         <v>117</v>
@@ -5071,24 +5071,24 @@
         <v>118</v>
       </c>
       <c r="E73" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F73" t="s">
         <v>119</v>
       </c>
       <c r="G73" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="H73" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I73" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B74" t="s">
         <v>52</v>
@@ -5100,24 +5100,24 @@
         <v>53</v>
       </c>
       <c r="E74" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F74" t="s">
         <v>54</v>
       </c>
       <c r="G74" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="H74" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I74" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B75" t="s">
         <v>71</v>
@@ -5129,24 +5129,24 @@
         <v>72</v>
       </c>
       <c r="E75" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F75" t="s">
         <v>73</v>
       </c>
       <c r="G75" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H75" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I75" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B76" t="s">
         <v>158</v>
@@ -5155,27 +5155,27 @@
         <v>89000000000</v>
       </c>
       <c r="D76" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E76" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F76" t="s">
         <v>159</v>
       </c>
       <c r="G76" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="H76" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I76" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B77" t="s">
         <v>120</v>
@@ -5187,24 +5187,24 @@
         <v>121</v>
       </c>
       <c r="E77" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F77" t="s">
         <v>122</v>
       </c>
       <c r="G77" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H77" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I77" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B78" t="s">
         <v>40</v>
@@ -5216,24 +5216,24 @@
         <v>41</v>
       </c>
       <c r="E78" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F78" t="s">
         <v>42</v>
       </c>
       <c r="G78" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="H78" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I78" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B79" t="s">
         <v>123</v>
@@ -5245,24 +5245,24 @@
         <v>124</v>
       </c>
       <c r="E79" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F79" t="s">
         <v>125</v>
       </c>
       <c r="G79" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H79" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I79" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B80" t="s">
         <v>172</v>
@@ -5271,56 +5271,56 @@
         <v>93000000000</v>
       </c>
       <c r="D80" t="s">
+        <v>695</v>
+      </c>
+      <c r="E80" t="s">
+        <v>696</v>
+      </c>
+      <c r="F80" t="s">
         <v>173</v>
       </c>
-      <c r="E80" t="s">
-        <v>581</v>
-      </c>
-      <c r="F80" t="s">
-        <v>174</v>
-      </c>
       <c r="G80" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="H80" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I80" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B81" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C81" s="1">
         <v>94000000000</v>
       </c>
       <c r="D81" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E81" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F81" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G81" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="H81" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I81" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B82" t="s">
         <v>156</v>
@@ -5329,27 +5329,27 @@
         <v>95000000000</v>
       </c>
       <c r="D82" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E82" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F82" t="s">
         <v>157</v>
       </c>
       <c r="G82" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="H82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I82" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B83" t="s">
         <v>15</v>
@@ -5361,24 +5361,24 @@
         <v>16</v>
       </c>
       <c r="E83" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F83" t="s">
         <v>17</v>
       </c>
       <c r="G83" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="H83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I83" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B84" t="s">
         <v>22</v>
@@ -5390,24 +5390,24 @@
         <v>23</v>
       </c>
       <c r="E84" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F84" t="s">
         <v>24</v>
       </c>
       <c r="G84" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="H84" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I84" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B85" t="s">
         <v>160</v>
@@ -5416,27 +5416,27 @@
         <v>98000000000</v>
       </c>
       <c r="D85" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E85" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F85" t="s">
         <v>161</v>
       </c>
       <c r="G85" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H85" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I85" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B86" t="s">
         <v>29</v>
@@ -5445,22 +5445,22 @@
         <v>99000000000</v>
       </c>
       <c r="D86" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E86" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F86" t="s">
         <v>30</v>
       </c>
       <c r="G86" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="H86" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I86" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>